<commit_message>
[update] improve emission calculator
</commit_message>
<xml_diff>
--- a/temp/data/EF_Table.xlsx
+++ b/temp/data/EF_Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hkt\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hkt\mvp\argo-ai-chatbot\temp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7511DC80-FB56-4014-9940-B22FEE6FFE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECBE654-71D8-4B8F-85FD-459F5D7FA1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B4C7DE61-2D6C-4D5C-80FF-3467FC6B8258}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="54">
   <si>
     <t>Continuous Flooding</t>
   </si>
@@ -180,6 +180,24 @@
   </si>
   <si>
     <t>scope</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Straw incorporated shortly</t>
+  </si>
+  <si>
+    <t>Straw incorporated long</t>
+  </si>
+  <si>
+    <t>Upland</t>
+  </si>
+  <si>
+    <t>Intermittent Flooding</t>
+  </si>
+  <si>
+    <t>Intermittently Flooded Fields</t>
   </si>
 </sst>
 </file>
@@ -601,882 +619,955 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE366BE-EB1F-4840-9FCE-B226F3F6D567}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
         <v>1.3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
         <v>0.8</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>1</v>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>0.5</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>1</v>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>0.2</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>1</v>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
         <v>0.1</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>1</v>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>1</v>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>1</v>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
         <v>0.05</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>1</v>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>1</v>
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
         <v>0.5</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>1</v>
+      <c r="F11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3">
         <v>18.3</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>1</v>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>1</v>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>1</v>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3">
         <v>20</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>1</v>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
         <v>0.01</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="H16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
         <v>0.01</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="3">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3">
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>1</v>
+      <c r="F18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3">
         <v>0.9</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>1</v>
+      <c r="D19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="3">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3">
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3">
         <v>0.15</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3">
         <v>2.68</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>1</v>
+      <c r="D22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
       </c>
       <c r="H22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="J22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K22" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="3">
         <v>2.31</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>1</v>
+      <c r="D23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="J23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K23" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="3">
         <v>0.52700000000000002</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>1</v>
+      <c r="D24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
       </c>
       <c r="H24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="J24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="3">
+      <c r="L24" s="3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{9684DFD4-B502-4DBD-B67E-9EA25A6B17AC}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{93D7575B-8E4F-4C65-A232-4B56E5FDE7F3}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{72946C30-47B6-419B-B53D-BF2C55889C85}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{D3AEA465-67D2-405C-BD71-6FB1B2B2A6B3}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{5FD232CD-BD66-4943-BE32-204FDD8B2433}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{63D36A89-27B6-4F1E-8917-3C4F4C368806}"/>
-    <hyperlink ref="I8" r:id="rId7" xr:uid="{430B834E-C618-47EF-ADFC-7B1FAE67B702}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{8B70DB80-D9AF-4CE2-A8E2-F87413382181}"/>
-    <hyperlink ref="I10" r:id="rId9" xr:uid="{8665878C-8B68-4249-8510-EF535DD3D3F0}"/>
-    <hyperlink ref="I11" r:id="rId10" xr:uid="{289C7364-7B7E-4F93-B16F-CE2B5FEB20B0}"/>
-    <hyperlink ref="I12" r:id="rId11" display="https://ecoinvent.org/" xr:uid="{CDA36BB4-C408-405D-B57B-7C02F0ADFEA7}"/>
-    <hyperlink ref="I13" r:id="rId12" display="https://ecoinvent.org/" xr:uid="{044CF230-5BF8-4909-B411-E403C2A9A8EA}"/>
-    <hyperlink ref="I14" r:id="rId13" display="https://ecoinvent.org/" xr:uid="{5F5C3544-CE54-4913-830D-7E38E43C92A4}"/>
-    <hyperlink ref="I15" r:id="rId14" display="https://ecoinvent.org/" xr:uid="{EBC11BD8-E564-49E0-AAF8-4B15231284BD}"/>
-    <hyperlink ref="I16" r:id="rId15" xr:uid="{E365AA3A-B4E9-4471-AC8C-FE9E80E7C8C3}"/>
-    <hyperlink ref="I17" r:id="rId16" xr:uid="{8C539124-7571-4273-82AB-98B00B749076}"/>
-    <hyperlink ref="I18" r:id="rId17" xr:uid="{9FCC2387-F8F3-4651-A7E9-2BA83BB3C093}"/>
-    <hyperlink ref="I19" r:id="rId18" xr:uid="{590BC1BD-70C6-4AD0-891F-922265CFEE7A}"/>
-    <hyperlink ref="I20" r:id="rId19" xr:uid="{432FF18F-5AC4-44BC-9898-1A9276CB38F5}"/>
-    <hyperlink ref="I21" r:id="rId20" xr:uid="{DA75B517-995F-4422-9CFE-CAE9DD6A6A8D}"/>
-    <hyperlink ref="I22" r:id="rId21" display="https://www.epa.gov/ghgemissions" xr:uid="{28558066-7014-4C55-8226-EDEB1E456328}"/>
-    <hyperlink ref="I23" r:id="rId22" display="https://www.epa.gov/ghgemissions" xr:uid="{16EB2AAA-5A48-4A61-BFDA-6C6EBFBA190D}"/>
-    <hyperlink ref="I24" r:id="rId23" display="https://www.iea.org/" xr:uid="{93F66913-7317-48E4-BE19-585A0F253D17}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{9684DFD4-B502-4DBD-B67E-9EA25A6B17AC}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{93D7575B-8E4F-4C65-A232-4B56E5FDE7F3}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{72946C30-47B6-419B-B53D-BF2C55889C85}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{D3AEA465-67D2-405C-BD71-6FB1B2B2A6B3}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{5FD232CD-BD66-4943-BE32-204FDD8B2433}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{63D36A89-27B6-4F1E-8917-3C4F4C368806}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{430B834E-C618-47EF-ADFC-7B1FAE67B702}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{8B70DB80-D9AF-4CE2-A8E2-F87413382181}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{8665878C-8B68-4249-8510-EF535DD3D3F0}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{289C7364-7B7E-4F93-B16F-CE2B5FEB20B0}"/>
+    <hyperlink ref="J12" r:id="rId11" display="https://ecoinvent.org/" xr:uid="{CDA36BB4-C408-405D-B57B-7C02F0ADFEA7}"/>
+    <hyperlink ref="J13" r:id="rId12" display="https://ecoinvent.org/" xr:uid="{044CF230-5BF8-4909-B411-E403C2A9A8EA}"/>
+    <hyperlink ref="J14" r:id="rId13" display="https://ecoinvent.org/" xr:uid="{5F5C3544-CE54-4913-830D-7E38E43C92A4}"/>
+    <hyperlink ref="J15" r:id="rId14" display="https://ecoinvent.org/" xr:uid="{EBC11BD8-E564-49E0-AAF8-4B15231284BD}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{E365AA3A-B4E9-4471-AC8C-FE9E80E7C8C3}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{8C539124-7571-4273-82AB-98B00B749076}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{9FCC2387-F8F3-4651-A7E9-2BA83BB3C093}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{590BC1BD-70C6-4AD0-891F-922265CFEE7A}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{432FF18F-5AC4-44BC-9898-1A9276CB38F5}"/>
+    <hyperlink ref="J21" r:id="rId20" xr:uid="{DA75B517-995F-4422-9CFE-CAE9DD6A6A8D}"/>
+    <hyperlink ref="J22" r:id="rId21" display="https://www.epa.gov/ghgemissions" xr:uid="{28558066-7014-4C55-8226-EDEB1E456328}"/>
+    <hyperlink ref="J23" r:id="rId22" display="https://www.epa.gov/ghgemissions" xr:uid="{16EB2AAA-5A48-4A61-BFDA-6C6EBFBA190D}"/>
+    <hyperlink ref="J24" r:id="rId23" display="https://www.iea.org/" xr:uid="{93F66913-7317-48E4-BE19-585A0F253D17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>